<commit_message>
Algorithm improve, data update
</commit_message>
<xml_diff>
--- a/Python/results.xlsx
+++ b/Python/results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="104">
   <si>
     <t>Cockroach Poker</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Jenga</t>
   </si>
   <si>
-    <t>11.99</t>
-  </si>
-  <si>
     <t>Deception: Murder in Hong Kong</t>
   </si>
   <si>
@@ -334,6 +331,12 @@
   </si>
   <si>
     <t>Games</t>
+  </si>
+  <si>
+    <t>Azul:Stained Glass of Sintra, Cryptid, Glux</t>
+  </si>
+  <si>
+    <t>Cockroach Poker, Wingspan, Junk-Art, Fog of Love, Mission: Red Planet (2nd edition)</t>
   </si>
 </sst>
 </file>
@@ -399,7 +402,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -422,11 +425,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -453,6 +467,9 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -738,7 +755,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,13 +765,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
         <v>71</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>72</v>
-      </c>
-      <c r="C1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -762,7 +779,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -817,7 +834,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>11</v>
@@ -850,158 +867,158 @@
         <v>16</v>
       </c>
       <c r="B10" s="2">
-        <v>7</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
+      </c>
+      <c r="C10" s="3">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2">
         <v>7</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2">
         <v>7</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2">
         <v>6</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="2">
+        <v>7</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="B14" s="2">
-        <v>6</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2">
+        <v>7</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="B15" s="2">
-        <v>6</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2">
         <v>5</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="2">
         <v>5</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="2">
         <v>4</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="2">
         <v>4</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="2">
         <v>4</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="2">
         <v>4</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="2">
         <v>4</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="2">
         <v>4</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="2">
         <v>3</v>
@@ -1012,145 +1029,145 @@
     </row>
     <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B25" s="2">
         <v>3</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="2">
+        <v>4</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="B26" s="2">
-        <v>3</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27" s="2">
         <v>3</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B28" s="2">
         <v>3</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="2">
+        <v>4</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="B29" s="2">
-        <v>3</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" s="2">
         <v>3</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B31" s="2">
         <v>2</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="2">
         <v>2</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="2">
+        <v>3</v>
+      </c>
+      <c r="C33" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="B33" s="2">
-        <v>2</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="2">
+        <v>3</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>63</v>
-      </c>
-      <c r="B34" s="2">
-        <v>2</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" s="2">
         <v>2</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B36" s="2">
         <v>1</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B37" s="2">
         <v>1</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1161,172 +1178,187 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A32"/>
+  <dimension ref="A1:A35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
-        <v>99</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>